<commit_message>
p24 and RLU titers calculated and cleaned
</commit_message>
<xml_diff>
--- a/experimental_validations/data/210122_p24_HAARVI_pvmuts.xlsx
+++ b/experimental_validations/data/210122_p24_HAARVI_pvmuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VEP_DMS_Barcode\plate_reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/fast/bloom_j/computational_notebooks/kdusenbu/2021/SARS-CoV-2-RBD_MAP_HAARVI_sera/experimental_validations/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D4002B3-F84F-4EAC-9399-167BD34815B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B32AB8-08C6-FC45-BC77-B61E3BD78DC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4485" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{42F3C59C-AE97-49F3-BBCB-B31F867B13FA}"/>
+    <workbookView xWindow="-31040" yWindow="4060" windowWidth="21920" windowHeight="15900" xr2:uid="{42F3C59C-AE97-49F3-BBCB-B31F867B13FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Tecan.At.Common, 3.9.1.0
 Tecan.At.Common.DocumentManagement, 3.9.1.0
@@ -112,7 +112,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
 MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="71">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -244,17 +244,110 @@
     <t>H</t>
   </si>
   <si>
-    <t>End Time:</t>
-  </si>
-  <si>
-    <t>1/22/2021 7:37:27 PM</t>
+    <t>StdCurve amounts p24</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>Std1</t>
+  </si>
+  <si>
+    <t>Std2</t>
+  </si>
+  <si>
+    <t>Virus1</t>
+  </si>
+  <si>
+    <t>media only</t>
+  </si>
+  <si>
+    <t>Virus2</t>
+  </si>
+  <si>
+    <t>Virus3</t>
+  </si>
+  <si>
+    <t>Virus4</t>
+  </si>
+  <si>
+    <t>Virus5</t>
+  </si>
+  <si>
+    <t>Virus6</t>
+  </si>
+  <si>
+    <t>Virus7</t>
+  </si>
+  <si>
+    <t>Virus8</t>
+  </si>
+  <si>
+    <t>Virus9</t>
+  </si>
+  <si>
+    <t>Virus10</t>
+  </si>
+  <si>
+    <t>Virus11</t>
+  </si>
+  <si>
+    <t>Virus12</t>
+  </si>
+  <si>
+    <t>Virus13</t>
+  </si>
+  <si>
+    <t>Virus14</t>
+  </si>
+  <si>
+    <t>Virus15</t>
+  </si>
+  <si>
+    <t>Virus16</t>
+  </si>
+  <si>
+    <t>Virus17</t>
+  </si>
+  <si>
+    <t>Virus18</t>
+  </si>
+  <si>
+    <t>Virus19</t>
+  </si>
+  <si>
+    <t>Virus20</t>
+  </si>
+  <si>
+    <t>Virus21</t>
+  </si>
+  <si>
+    <t>Virus22</t>
+  </si>
+  <si>
+    <t>Virus23</t>
+  </si>
+  <si>
+    <t>Avg reps</t>
+  </si>
+  <si>
+    <t>grey-filled is bg average</t>
+  </si>
+  <si>
+    <t>Avg-bg</t>
+  </si>
+  <si>
+    <t>Calc from trendline</t>
+  </si>
+  <si>
+    <t>Times 100,000 dilutionfactor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,10 +374,16 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,61 +434,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7FFFD4"/>
+        <fgColor rgb="FF808080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6495ED"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF32CD32"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9ACD32"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8FBC8B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDEB887"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4A460"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD2691E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,11 +470,14 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,6 +500,985 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>p24_std</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.4398512685914264E-2"/>
+                  <c:y val="-0.16708333333333333"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$25:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$L$35:$L$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1051250044256449</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55162500776350498</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26912500895559788</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1361249927431345</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3275003805756569E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2124998047947884E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1524999514222145E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FC35-9B4B-B8FC-8BDC0684F8E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2074630336"/>
+        <c:axId val="2074628480"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2074630336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2074628480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2074628480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2074630336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBE35668-DD11-CF44-A850-BFBD637712BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -739,13 +1778,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9412B28-6A01-47CD-969E-DA41C36E5222}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="R55" sqref="R55:R61"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -761,7 +1802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -769,7 +1810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -777,7 +1818,7 @@
         <v>44218</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -785,7 +1826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -793,7 +1834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -801,7 +1842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -809,25 +1850,137 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3">
+        <v>2</v>
+      </c>
+      <c r="N13" s="3">
+        <v>3</v>
+      </c>
+      <c r="O13" s="3">
+        <v>4</v>
+      </c>
+      <c r="P13" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>6</v>
+      </c>
+      <c r="R13" s="3">
+        <v>7</v>
+      </c>
+      <c r="S13" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" t="s">
+        <v>42</v>
+      </c>
+      <c r="P14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>51</v>
+      </c>
+      <c r="R14" t="s">
+        <v>59</v>
+      </c>
+      <c r="S14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M15" t="s">
+        <v>41</v>
+      </c>
+      <c r="N15" t="s">
+        <v>44</v>
+      </c>
+      <c r="O15" t="s">
+        <v>44</v>
+      </c>
+      <c r="P15" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>52</v>
+      </c>
+      <c r="R15" t="s">
+        <v>60</v>
+      </c>
+      <c r="S15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L16" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" t="s">
+        <v>45</v>
+      </c>
+      <c r="O16" t="s">
+        <v>45</v>
+      </c>
+      <c r="P16" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>53</v>
+      </c>
+      <c r="R16" t="s">
+        <v>61</v>
+      </c>
+      <c r="S16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -837,16 +1990,70 @@
       <c r="F17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" t="s">
+        <v>41</v>
+      </c>
+      <c r="N17" t="s">
+        <v>46</v>
+      </c>
+      <c r="O17" t="s">
+        <v>46</v>
+      </c>
+      <c r="P17" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>54</v>
+      </c>
+      <c r="R17" t="s">
+        <v>62</v>
+      </c>
+      <c r="S17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="E18">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" t="s">
+        <v>47</v>
+      </c>
+      <c r="O18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P18" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>55</v>
+      </c>
+      <c r="R18" t="s">
+        <v>63</v>
+      </c>
+      <c r="S18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -856,29 +2063,116 @@
       <c r="F19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19" t="s">
+        <v>48</v>
+      </c>
+      <c r="P19" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>56</v>
+      </c>
+      <c r="R19" t="s">
+        <v>64</v>
+      </c>
+      <c r="S19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" t="s">
+        <v>41</v>
+      </c>
+      <c r="N20" t="s">
+        <v>49</v>
+      </c>
+      <c r="O20" t="s">
+        <v>49</v>
+      </c>
+      <c r="P20" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>57</v>
+      </c>
+      <c r="R20" t="s">
+        <v>65</v>
+      </c>
+      <c r="S20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L21" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" t="s">
+        <v>43</v>
+      </c>
+      <c r="N21" t="s">
+        <v>50</v>
+      </c>
+      <c r="O21" t="s">
+        <v>50</v>
+      </c>
+      <c r="P21" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>58</v>
+      </c>
+      <c r="R21" t="s">
+        <v>43</v>
+      </c>
+      <c r="S21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>38</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -906,8 +2200,35 @@
       <c r="I24" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1</v>
+      </c>
+      <c r="M24" s="3">
+        <v>2</v>
+      </c>
+      <c r="N24" s="3">
+        <v>3</v>
+      </c>
+      <c r="O24" s="3">
+        <v>4</v>
+      </c>
+      <c r="P24" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>6</v>
+      </c>
+      <c r="R24" s="3">
+        <v>7</v>
+      </c>
+      <c r="S24" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
@@ -935,8 +2256,30 @@
       <c r="I25">
         <v>0.11140000075101852</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25">
+        <f>AVERAGE(B25:C25)</f>
+        <v>1.1825000047683716</v>
+      </c>
+      <c r="N25">
+        <f>AVERAGE(D25:E25)</f>
+        <v>0.17125000059604645</v>
+      </c>
+      <c r="P25">
+        <f>AVERAGE(F25:G25)</f>
+        <v>0.27100000530481339</v>
+      </c>
+      <c r="R25">
+        <f>AVERAGE(H25:I25)</f>
+        <v>0.10990000143647194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>31</v>
       </c>
@@ -964,8 +2307,31 @@
       <c r="I26">
         <v>0.14890000224113464</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <f>J25/2</f>
+        <v>50</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ref="L26:R32" si="0">AVERAGE(B26:C26)</f>
+        <v>0.62900000810623169</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>0.19305000454187393</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="0"/>
+        <v>0.17219999432563782</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="0"/>
+        <v>0.1445000022649765</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
@@ -993,8 +2359,31 @@
       <c r="I27">
         <v>0.27570000290870667</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <f t="shared" ref="J27:J31" si="1">J26/2</f>
+        <v>25</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>0.34650000929832458</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>0.21709999442100525</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>0.11890000104904175</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="0"/>
+        <v>0.25919999927282333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
@@ -1022,8 +2411,31 @@
       <c r="I28">
         <v>0.18639999628067017</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>0.21349999308586121</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>0.18609999865293503</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>0.17674999684095383</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="0"/>
+        <v>0.17314999550580978</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
@@ -1051,8 +2463,31 @@
       <c r="I29">
         <v>0.18039999902248383</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>0.14065000414848328</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>0.15700000524520874</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="0"/>
+        <v>0.16609999537467957</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="0"/>
+        <v>0.22070000320672989</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>35</v>
       </c>
@@ -1080,8 +2515,31 @@
       <c r="I30">
         <v>0.17170000076293945</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>3.125</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>0.10949999839067459</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>0.18930000066757202</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>0.12834999710321426</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="0"/>
+        <v>0.17949999868869781</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
@@ -1109,8 +2567,31 @@
       <c r="I31">
         <v>0.37709999084472656</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>1.5625</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>8.8899999856948853E-2</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>0.15789999812841415</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="0"/>
+        <v>0.14549999684095383</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="0"/>
+        <v>0.38749998807907104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
@@ -1138,18 +2619,576 @@
       <c r="I32">
         <v>8.1799998879432678E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>39</v>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L32" s="4">
+        <f>AVERAGE(B32:C32,H32:I32)</f>
+        <v>7.7375000342726707E-2</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>0.16295000165700912</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>0.15590000152587891</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="K34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L34" s="3">
+        <v>1</v>
+      </c>
+      <c r="M34" s="3">
+        <v>2</v>
+      </c>
+      <c r="N34" s="3">
+        <v>3</v>
+      </c>
+      <c r="O34" s="3">
+        <v>4</v>
+      </c>
+      <c r="P34" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>6</v>
+      </c>
+      <c r="R34" s="3">
+        <v>7</v>
+      </c>
+      <c r="S34" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L35">
+        <f>L25-$L$32</f>
+        <v>1.1051250044256449</v>
+      </c>
+      <c r="N35">
+        <f>N25-$L$32</f>
+        <v>9.387500025331974E-2</v>
+      </c>
+      <c r="P35">
+        <f>P25-$L$32</f>
+        <v>0.19362500496208668</v>
+      </c>
+      <c r="R35">
+        <f>R25-$L$32</f>
+        <v>3.2525001093745232E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K36" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36">
+        <f t="shared" ref="L36:N42" si="2">L26-$L$32</f>
+        <v>0.55162500776350498</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>0.11567500419914722</v>
+      </c>
+      <c r="P36">
+        <f t="shared" ref="P36" si="3">P26-$L$32</f>
+        <v>9.482499398291111E-2</v>
+      </c>
+      <c r="R36">
+        <f t="shared" ref="R36" si="4">R26-$L$32</f>
+        <v>6.7125001922249794E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B37" s="2"/>
+      <c r="K37" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>0.26912500895559788</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>0.13972499407827854</v>
+      </c>
+      <c r="P37">
+        <f t="shared" ref="P37" si="5">P27-$L$32</f>
+        <v>4.1525000706315041E-2</v>
+      </c>
+      <c r="R37">
+        <f t="shared" ref="R37" si="6">R27-$L$32</f>
+        <v>0.18182499893009663</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>0.1361249927431345</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>0.10872499831020832</v>
+      </c>
+      <c r="P38">
+        <f t="shared" ref="P38" si="7">P28-$L$32</f>
+        <v>9.9374996498227119E-2</v>
+      </c>
+      <c r="R38">
+        <f t="shared" ref="R38" si="8">R28-$L$32</f>
+        <v>9.5774995163083076E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K39" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>6.3275003805756569E-2</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>7.9625004902482033E-2</v>
+      </c>
+      <c r="P39">
+        <f t="shared" ref="P39" si="9">P29-$L$32</f>
+        <v>8.8724995031952858E-2</v>
+      </c>
+      <c r="R39">
+        <f t="shared" ref="R39" si="10">R29-$L$32</f>
+        <v>0.14332500286400318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K40" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="2"/>
+        <v>3.2124998047947884E-2</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>0.11192500032484531</v>
+      </c>
+      <c r="P40">
+        <f t="shared" ref="P40" si="11">P30-$L$32</f>
+        <v>5.0974996760487556E-2</v>
+      </c>
+      <c r="R40">
+        <f t="shared" ref="R40" si="12">R30-$L$32</f>
+        <v>0.10212499834597111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>1.1524999514222145E-2</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="2"/>
+        <v>8.0524997785687447E-2</v>
+      </c>
+      <c r="P41">
+        <f t="shared" ref="P41" si="13">P31-$L$32</f>
+        <v>6.8124996498227119E-2</v>
+      </c>
+      <c r="R41">
+        <f t="shared" ref="R41" si="14">R31-$L$32</f>
+        <v>0.31012498773634434</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>8.5575001314282417E-2</v>
+      </c>
+      <c r="P42">
+        <f t="shared" ref="P42" si="15">P32-$L$32</f>
+        <v>7.8525001183152199E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K44" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L44" s="3">
+        <v>1</v>
+      </c>
+      <c r="M44" s="3">
+        <v>2</v>
+      </c>
+      <c r="N44" s="3">
+        <v>3</v>
+      </c>
+      <c r="O44" s="3">
+        <v>4</v>
+      </c>
+      <c r="P44" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>6</v>
+      </c>
+      <c r="R44" s="3">
+        <v>7</v>
+      </c>
+      <c r="S44" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K45" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L45">
+        <f>(L35+0.0048)/0.0111</f>
+        <v>99.993243641949974</v>
+      </c>
+      <c r="N45">
+        <f>(N35+0.0048)/0.0111</f>
+        <v>8.8896396624612368</v>
+      </c>
+      <c r="P45">
+        <f>(P35+0.0048)/0.0111</f>
+        <v>17.87612657316096</v>
+      </c>
+      <c r="R45">
+        <f>(R35+0.0048)/0.0111</f>
+        <v>3.3626127111482189</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K46" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L46">
+        <f t="shared" ref="L46:N52" si="16">(L36+0.0048)/0.0111</f>
+        <v>50.128379077793241</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="16"/>
+        <v>10.853603981905154</v>
+      </c>
+      <c r="P46">
+        <f t="shared" ref="P46" si="17">(P36+0.0048)/0.0111</f>
+        <v>8.9752246831451448</v>
+      </c>
+      <c r="R46">
+        <f t="shared" ref="R46" si="18">(R36+0.0048)/0.0111</f>
+        <v>6.4797299029053868</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="16"/>
+        <v>24.677928734738551</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="16"/>
+        <v>13.020269736781851</v>
+      </c>
+      <c r="P47">
+        <f t="shared" ref="P47" si="19">(P37+0.0048)/0.0111</f>
+        <v>4.173423487055409</v>
+      </c>
+      <c r="R47">
+        <f t="shared" ref="R47" si="20">(R37+0.0048)/0.0111</f>
+        <v>16.813062966675371</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="16"/>
+        <v>12.695945292174278</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="16"/>
+        <v>10.227477325243992</v>
+      </c>
+      <c r="P48">
+        <f t="shared" ref="P48" si="21">(P38+0.0048)/0.0111</f>
+        <v>9.3851348196601005</v>
+      </c>
+      <c r="R48">
+        <f t="shared" ref="R48" si="22">(R38+0.0048)/0.0111</f>
+        <v>9.0608103750525295</v>
+      </c>
+    </row>
+    <row r="49" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K49" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="16"/>
+        <v>6.1328832257438348</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="16"/>
+        <v>7.6058562975209032</v>
+      </c>
+      <c r="P49">
+        <f t="shared" ref="P49" si="23">(P39+0.0048)/0.0111</f>
+        <v>8.4256752281038612</v>
+      </c>
+      <c r="R49">
+        <f t="shared" ref="R49" si="24">(R39+0.0048)/0.0111</f>
+        <v>13.344594852612898</v>
+      </c>
+    </row>
+    <row r="50" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K50" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="16"/>
+        <v>3.3265764007160255</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="16"/>
+        <v>10.515765795031109</v>
+      </c>
+      <c r="P50">
+        <f t="shared" ref="P50" si="25">(P40+0.0048)/0.0111</f>
+        <v>5.0247744829268068</v>
+      </c>
+      <c r="R50">
+        <f t="shared" ref="R50" si="26">(R40+0.0048)/0.0111</f>
+        <v>9.6328827338712699</v>
+      </c>
+    </row>
+    <row r="51" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K51" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="16"/>
+        <v>1.4707206769569499</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="16"/>
+        <v>7.6869367374493187</v>
+      </c>
+      <c r="P51">
+        <f t="shared" ref="P51" si="27">(P41+0.0048)/0.0111</f>
+        <v>6.5698195043447853</v>
+      </c>
+      <c r="R51">
+        <f t="shared" ref="R51" si="28">(R41+0.0048)/0.0111</f>
+        <v>28.371620516787779</v>
+      </c>
+    </row>
+    <row r="52" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K52" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="16"/>
+        <v>8.1418920102957131</v>
+      </c>
+      <c r="P52">
+        <f t="shared" ref="P52" si="29">(P42+0.0048)/0.0111</f>
+        <v>7.5067568633470447</v>
+      </c>
+    </row>
+    <row r="54" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K54" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L54" s="3">
+        <v>1</v>
+      </c>
+      <c r="M54" s="3">
+        <v>2</v>
+      </c>
+      <c r="N54" s="3">
+        <v>3</v>
+      </c>
+      <c r="O54" s="3">
+        <v>4</v>
+      </c>
+      <c r="P54" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>6</v>
+      </c>
+      <c r="R54" s="3">
+        <v>7</v>
+      </c>
+      <c r="S54" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K55" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N55">
+        <f>N45*100000</f>
+        <v>888963.96624612366</v>
+      </c>
+      <c r="P55">
+        <f>P45*100000</f>
+        <v>1787612.6573160959</v>
+      </c>
+      <c r="R55">
+        <f>R45*100000</f>
+        <v>336261.2711148219</v>
+      </c>
+    </row>
+    <row r="56" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K56" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N56">
+        <f t="shared" ref="N56:P62" si="30">N46*100000</f>
+        <v>1085360.3981905153</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="30"/>
+        <v>897522.4683145145</v>
+      </c>
+      <c r="R56">
+        <f t="shared" ref="R56" si="31">R46*100000</f>
+        <v>647972.99029053864</v>
+      </c>
+    </row>
+    <row r="57" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="30"/>
+        <v>1302026.9736781851</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="30"/>
+        <v>417342.34870554088</v>
+      </c>
+      <c r="R57">
+        <f t="shared" ref="R57" si="32">R47*100000</f>
+        <v>1681306.2966675372</v>
+      </c>
+    </row>
+    <row r="58" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="30"/>
+        <v>1022747.7325243992</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="30"/>
+        <v>938513.48196601006</v>
+      </c>
+      <c r="R58">
+        <f t="shared" ref="R58" si="33">R48*100000</f>
+        <v>906081.03750525299</v>
+      </c>
+    </row>
+    <row r="59" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K59" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="30"/>
+        <v>760585.62975209032</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="30"/>
+        <v>842567.52281038614</v>
+      </c>
+      <c r="R59">
+        <f t="shared" ref="R59" si="34">R49*100000</f>
+        <v>1334459.4852612899</v>
+      </c>
+    </row>
+    <row r="60" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K60" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="30"/>
+        <v>1051576.5795031108</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="30"/>
+        <v>502477.44829268067</v>
+      </c>
+      <c r="R60">
+        <f t="shared" ref="R60" si="35">R50*100000</f>
+        <v>963288.27338712697</v>
+      </c>
+    </row>
+    <row r="61" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="30"/>
+        <v>768693.67374493182</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="30"/>
+        <v>656981.95043447858</v>
+      </c>
+      <c r="R61">
+        <f t="shared" ref="R61" si="36">R51*100000</f>
+        <v>2837162.0516787777</v>
+      </c>
+    </row>
+    <row r="62" spans="11:19" x14ac:dyDescent="0.2">
+      <c r="K62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="30"/>
+        <v>814189.20102957136</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="30"/>
+        <v>750675.68633470451</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1159,7 +3198,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>